<commit_message>
added some columns to the RMMM plan
</commit_message>
<xml_diff>
--- a/trunk/docs/Risk Management/Risk Managment(RMMM).xlsx
+++ b/trunk/docs/Risk Management/Risk Managment(RMMM).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
   <si>
     <t>Risk Mitigation, Monitoring and Management Plan</t>
   </si>
@@ -114,9 +114,6 @@
     <t xml:space="preserve">Adopt good HCI practices </t>
   </si>
   <si>
-    <t>Test the GUI before the final deployment. Test must include a wide range of user (novice and experts).</t>
-  </si>
-  <si>
     <t>Understand the difficulties the user is facing and modify the GUI in accordance to that</t>
   </si>
   <si>
@@ -129,15 +126,9 @@
     <t>Try and maintain regular communication with the client.</t>
   </si>
   <si>
-    <t>People don’t work well together</t>
-  </si>
-  <si>
     <t>Staff</t>
   </si>
   <si>
-    <t>Team leader to find out early on how does the team look and decided whether a change is needed.</t>
-  </si>
-  <si>
     <t>Get regular feedback from members to see if there are problems.</t>
   </si>
   <si>
@@ -184,6 +175,60 @@
   </si>
   <si>
     <t>Check if the new requirements require re planning and reassigning tasks to the team.</t>
+  </si>
+  <si>
+    <t>Loss of data</t>
+  </si>
+  <si>
+    <t>While team member are working on their own copy of the applciation, they might encounter loss of data</t>
+  </si>
+  <si>
+    <t>Once you have a working copy, commit to the repositry</t>
+  </si>
+  <si>
+    <t>Get the team member who was working on that lost data to start re-developing whats lost immediatly, assign another team member if help is needed.</t>
+  </si>
+  <si>
+    <t>Miscommunication with the client</t>
+  </si>
+  <si>
+    <t>Miss understanding that clients requirments can ocurr as project goes on.</t>
+  </si>
+  <si>
+    <t>Always check with the client whether the project is meeting their needs and if they are happy with what has been developed already.</t>
+  </si>
+  <si>
+    <t>Find out what has been misunderstood and re-plan to meet the client needs.</t>
+  </si>
+  <si>
+    <t>During the protypes demonstration with the client, check with client if everything is on track.</t>
+  </si>
+  <si>
+    <t>Standards</t>
+  </si>
+  <si>
+    <t>Deviation from software engineering standards</t>
+  </si>
+  <si>
+    <t>be as complete and accurate as possible to ensure that work will conform to</t>
+  </si>
+  <si>
+    <t>expressed software engineering standards</t>
+  </si>
+  <si>
+    <t>With the progress of the develpoment it is possible to lose track and start deviating from the common and known software engineering standards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tehnical reviews to be done during major milestones to ensure that the project is in line with established software engineering standards </t>
+  </si>
+  <si>
+    <t>steps must be taken back as soon as the deviations are spotted, and try and guide and the project back to meet the standards.</t>
+  </si>
+  <si>
+    <t>All relevant documents must be complete and as accurate as possible to ensure they conform with common software enigneering standards</t>
+  </si>
+  <si>
+    <t>Test the GUI before the final deployment. Tests must include a wide range of users (novice and expert).</t>
   </si>
 </sst>
 </file>
@@ -259,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -359,11 +404,59 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -371,17 +464,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -433,14 +520,41 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,15 +850,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" customWidth="1"/>
@@ -754,253 +868,331 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="26" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="67.5" customHeight="1" thickBot="1">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="67.5" customHeight="1" thickBot="1">
+      <c r="A4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="67.5" customHeight="1" thickBot="1">
+      <c r="A5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="71.25" customHeight="1" thickBot="1">
+      <c r="A6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="63.75" customHeight="1" thickBot="1">
+      <c r="A7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="57" customHeight="1" thickBot="1">
+      <c r="A8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="52.5" customHeight="1" thickBot="1">
+      <c r="A9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="111" customHeight="1" thickBot="1">
+      <c r="A10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="67.5" customHeight="1" thickBot="1">
+      <c r="A11" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="67.5" customHeight="1" thickBot="1">
-      <c r="A4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="15" t="s">
+      <c r="F11" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
+      <c r="A12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="54.75" customHeight="1" thickBot="1">
+      <c r="A13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="71.25" customHeight="1" thickBot="1">
-      <c r="A5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A6" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="57" customHeight="1" thickBot="1">
-      <c r="A7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="39" thickBot="1">
-      <c r="A8" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="E13" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="F13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="54.75" customHeight="1" thickBot="1">
-      <c r="A10" s="11" t="s">
+      <c r="G13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="20" t="s">
+      <c r="H13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="F11" s="1"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fixed second to last column mistakes..
</commit_message>
<xml_diff>
--- a/trunk/docs/Risk Management/Risk Managment(RMMM).xlsx
+++ b/trunk/docs/Risk Management/Risk Managment(RMMM).xlsx
@@ -204,9 +204,6 @@
     <t>During the protypes demonstration with the client, check with client if everything is on track.</t>
   </si>
   <si>
-    <t>Standards</t>
-  </si>
-  <si>
     <t>Deviation from software engineering standards</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
   </si>
   <si>
     <t>Test the GUI before the final deployment. Tests must include a wide range of users (novice and expert).</t>
+  </si>
+  <si>
+    <t>People don't work well together</t>
   </si>
 </sst>
 </file>
@@ -544,6 +544,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -552,9 +555,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -868,16 +868,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="30.75" customHeight="1" thickBot="1">
       <c r="A2" s="25" t="s">
@@ -1055,7 +1055,7 @@
         <v>31</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>32</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="10" spans="1:8" ht="111" customHeight="1" thickBot="1">
       <c r="A10" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>16</v>
@@ -1101,16 +1101,16 @@
         <v>22</v>
       </c>
       <c r="E10" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" s="30" t="s">
+      <c r="H10" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="67.5" customHeight="1" thickBot="1">
@@ -1130,7 +1130,7 @@
         <v>54</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>55</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="12" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
       <c r="A12" s="9" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>36</v>
@@ -1156,7 +1156,7 @@
         <v>45</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>37</v>

</xml_diff>